<commit_message>
aggiunta del foglio di calcolo VariableCostsBudget
</commit_message>
<xml_diff>
--- a/Progetto_sdg.xlsx
+++ b/Progetto_sdg.xlsx
@@ -5,23 +5,24 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marco\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marco\Documents\GitHub\script-analisi-scostamenti\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1540652D-F389-42BB-888E-7E941DBA606F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76F1F44C-1D14-441B-94DF-A75949399CC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CE 21-22" sheetId="3" r:id="rId1"/>
     <sheet name="Ricavi" sheetId="1" r:id="rId2"/>
     <sheet name="RicaviBudget" sheetId="7" r:id="rId3"/>
     <sheet name="VariableCosts" sheetId="4" r:id="rId4"/>
-    <sheet name="FixedCosts" sheetId="5" r:id="rId5"/>
-    <sheet name="Others" sheetId="6" r:id="rId6"/>
+    <sheet name="VariableCostsBudget" sheetId="8" r:id="rId5"/>
+    <sheet name="FixedCosts" sheetId="5" r:id="rId6"/>
+    <sheet name="Others" sheetId="6" r:id="rId7"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId7"/>
+    <externalReference r:id="rId8"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="238">
   <si>
     <t>MP1</t>
   </si>
@@ -721,6 +722,117 @@
   </si>
   <si>
     <t>Totale Ricavi Budget</t>
+  </si>
+  <si>
+    <t>Voce di costo</t>
+  </si>
+  <si>
+    <t>Formula/base di cacolo</t>
+  </si>
+  <si>
+    <t>Valore Budget (€)</t>
+  </si>
+  <si>
+    <t>Famiglia</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Polveri P, comsumi energia/metano diversi</t>
+  </si>
+  <si>
+    <t>Polveri V, comsumi medi diversi</t>
+  </si>
+  <si>
+    <t>Polveri A, consumi diversi dai primi due</t>
+  </si>
+  <si>
+    <t>PF V</t>
+  </si>
+  <si>
+    <t>PF A</t>
+  </si>
+  <si>
+    <t>Totale PF</t>
+  </si>
+  <si>
+    <t>quantita budget (kg)</t>
+  </si>
+  <si>
+    <t>Quantità Budget (ton)</t>
+  </si>
+  <si>
+    <t>Costo energia totale 2021</t>
+  </si>
+  <si>
+    <t>% elettricità</t>
+  </si>
+  <si>
+    <t>% metano</t>
+  </si>
+  <si>
+    <t>kWh 2021</t>
+  </si>
+  <si>
+    <t>smc metano 2021</t>
+  </si>
+  <si>
+    <t>Costo elettricità 2021</t>
+  </si>
+  <si>
+    <t>Costo Metano 2021</t>
+  </si>
+  <si>
+    <t>Prezzo €/kWh 2021</t>
+  </si>
+  <si>
+    <t>Prezzo €/smc 2021</t>
+  </si>
+  <si>
+    <t>Aumento Elettricità 2022</t>
+  </si>
+  <si>
+    <t>Aumento Metano 2022</t>
+  </si>
+  <si>
+    <t>Prezzo €/kWh 2022</t>
+  </si>
+  <si>
+    <t>Prezzo €/smc 2022</t>
+  </si>
+  <si>
+    <t>=(ton PF A*0,93 + ton PF V*0,64)*prezzo smc 2022</t>
+  </si>
+  <si>
+    <t>=(ton P*140 + ton V*60 + ton A*65 + 3.300.000)*prezzo kWh 2022</t>
+  </si>
+  <si>
+    <t>Costo metano</t>
+  </si>
+  <si>
+    <t>Costo energia elettrica</t>
+  </si>
+  <si>
+    <t>Materiali di consumo</t>
+  </si>
+  <si>
+    <t>Pulizia e smaltimento rifiuti</t>
+  </si>
+  <si>
+    <t>Trasporti vendita</t>
+  </si>
+  <si>
+    <t>Provvigioni su vendite</t>
+  </si>
+  <si>
+    <t>Totale costi variabili</t>
   </si>
 </sst>
 </file>
@@ -1602,6 +1714,7 @@
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="165" fontId="13" fillId="2" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1635,7 +1748,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="19">
     <cellStyle name="Euro" xfId="16" xr:uid="{6609C029-AE67-4DF2-BB38-0E304B6F97A8}"/>
@@ -2549,8 +2661,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C09E9022-8714-451A-AC8C-ADBBD3500E3D}">
   <dimension ref="B1:J62"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A30" zoomScale="92" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8:D10"/>
+    <sheetView showGridLines="0" zoomScale="92" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2567,23 +2679,23 @@
   <sheetData>
     <row r="1" spans="2:10" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="95" t="s">
+      <c r="B2" s="96" t="s">
         <v>139</v>
       </c>
-      <c r="C2" s="96"/>
-      <c r="E2" s="95" t="s">
+      <c r="C2" s="97"/>
+      <c r="E2" s="96" t="s">
         <v>139</v>
       </c>
-      <c r="F2" s="96"/>
+      <c r="F2" s="97"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="93" t="s">
+      <c r="B3" s="94" t="s">
         <v>169</v>
       </c>
       <c r="C3" s="42" t="s">
         <v>65</v>
       </c>
-      <c r="E3" s="97" t="s">
+      <c r="E3" s="98" t="s">
         <v>170</v>
       </c>
       <c r="F3" s="80" t="s">
@@ -2591,11 +2703,11 @@
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="94"/>
+      <c r="B4" s="95"/>
       <c r="C4" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="E4" s="94"/>
+      <c r="E4" s="95"/>
       <c r="F4" s="43" t="s">
         <v>66</v>
       </c>
@@ -3237,8 +3349,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:XFD1048576"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A48" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:Q84"/>
+    <sheetView showGridLines="0" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3263,24 +3375,24 @@
   <sheetData>
     <row r="1" spans="1:17" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="98" t="s">
+      <c r="B2" s="99" t="s">
         <v>162</v>
       </c>
-      <c r="C2" s="99"/>
-      <c r="D2" s="99"/>
-      <c r="E2" s="99"/>
-      <c r="F2" s="100"/>
+      <c r="C2" s="100"/>
+      <c r="D2" s="100"/>
+      <c r="E2" s="100"/>
+      <c r="F2" s="101"/>
       <c r="H2" s="59"/>
-      <c r="J2" s="98" t="s">
+      <c r="J2" s="99" t="s">
         <v>64</v>
       </c>
-      <c r="K2" s="99"/>
-      <c r="L2" s="99"/>
-      <c r="M2" s="99"/>
-      <c r="N2" s="99"/>
-      <c r="O2" s="99"/>
-      <c r="P2" s="99"/>
-      <c r="Q2" s="100"/>
+      <c r="K2" s="100"/>
+      <c r="L2" s="100"/>
+      <c r="M2" s="100"/>
+      <c r="N2" s="100"/>
+      <c r="O2" s="100"/>
+      <c r="P2" s="100"/>
+      <c r="Q2" s="101"/>
     </row>
     <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="54" t="s">
@@ -6344,10 +6456,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EAEFA6D-2B43-44D4-9785-BA525C9ED11E}">
-  <dimension ref="B2:G67"/>
+  <dimension ref="B2:H67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="F75" sqref="F75"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H45" sqref="H45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6356,10 +6468,11 @@
     <col min="3" max="3" width="10" customWidth="1"/>
     <col min="4" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="38.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>110</v>
       </c>
@@ -6376,10 +6489,13 @@
         <v>198</v>
       </c>
       <c r="G2" t="s">
+        <v>204</v>
+      </c>
+      <c r="H2" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" t="str">
         <f>Ricavi!J4</f>
         <v>MP1</v>
@@ -6397,11 +6513,11 @@
         <v>0.93</v>
       </c>
       <c r="F3">
-        <f>D3*E3</f>
+        <f t="shared" ref="F3:F34" si="0">D3*E3</f>
         <v>44640</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" t="str">
         <f>Ricavi!J5</f>
         <v>MP2</v>
@@ -6419,11 +6535,11 @@
         <v>4</v>
       </c>
       <c r="F4">
-        <f>D4*E4</f>
+        <f t="shared" si="0"/>
         <v>2800</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" t="str">
         <f>Ricavi!J6</f>
         <v>MP3</v>
@@ -6441,11 +6557,11 @@
         <v>2.4</v>
       </c>
       <c r="F5">
-        <f>D5*E5</f>
+        <f t="shared" si="0"/>
         <v>2640</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" t="str">
         <f>Ricavi!J7</f>
         <v>MP4</v>
@@ -6463,11 +6579,11 @@
         <v>4</v>
       </c>
       <c r="F6">
-        <f>D6*E6</f>
+        <f t="shared" si="0"/>
         <v>500</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" t="str">
         <f>Ricavi!J8</f>
         <v>MP5</v>
@@ -6485,11 +6601,11 @@
         <v>2.9058441558441559</v>
       </c>
       <c r="F7">
-        <f>D7*E7</f>
+        <f t="shared" si="0"/>
         <v>5593.75</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" t="str">
         <f>Ricavi!J9</f>
         <v>MP6</v>
@@ -6507,11 +6623,11 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="F8">
-        <f>D8*E8</f>
+        <f t="shared" si="0"/>
         <v>550</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" t="str">
         <f>Ricavi!J10</f>
         <v>MP7</v>
@@ -6529,11 +6645,11 @@
         <v>4.62</v>
       </c>
       <c r="F9">
-        <f>D9*E9</f>
+        <f t="shared" si="0"/>
         <v>9240</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" t="str">
         <f>Ricavi!J11</f>
         <v>MP8</v>
@@ -6551,11 +6667,11 @@
         <v>2.65</v>
       </c>
       <c r="F10">
-        <f>D10*E10</f>
+        <f t="shared" si="0"/>
         <v>2650</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" t="str">
         <f>Ricavi!J12</f>
         <v>MP9</v>
@@ -6573,11 +6689,11 @@
         <v>0.19</v>
       </c>
       <c r="F11">
-        <f>D11*E11</f>
+        <f t="shared" si="0"/>
         <v>1330</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" t="str">
         <f>Ricavi!J13</f>
         <v>MP10</v>
@@ -6595,11 +6711,11 @@
         <v>0.50710643771654074</v>
       </c>
       <c r="F12">
-        <f>D12*E12</f>
+        <f t="shared" si="0"/>
         <v>17680.975899999998</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" t="str">
         <f>Ricavi!J14</f>
         <v>MP11</v>
@@ -6617,11 +6733,11 @@
         <v>7.4104528564263887</v>
       </c>
       <c r="F13">
-        <f>D13*E13</f>
+        <f t="shared" si="0"/>
         <v>104021.416</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" t="str">
         <f>Ricavi!J15</f>
         <v>MP12</v>
@@ -6639,11 +6755,11 @@
         <v>1.4275735294117646</v>
       </c>
       <c r="F14">
-        <f>D14*E14</f>
+        <f t="shared" si="0"/>
         <v>2718.1</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" t="str">
         <f>Ricavi!J16</f>
         <v>MP13</v>
@@ -6661,11 +6777,11 @@
         <v>13</v>
       </c>
       <c r="F15">
-        <f>D15*E15</f>
+        <f t="shared" si="0"/>
         <v>1950</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" t="str">
         <f>Ricavi!J17</f>
         <v>MP14</v>
@@ -6683,11 +6799,11 @@
         <v>13.5</v>
       </c>
       <c r="F16">
-        <f>D16*E16</f>
+        <f t="shared" si="0"/>
         <v>270</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" t="str">
         <f>Ricavi!J18</f>
         <v>PCL1</v>
@@ -6705,11 +6821,11 @@
         <v>0.11065878100870709</v>
       </c>
       <c r="F17">
-        <f>D17*E17</f>
+        <f t="shared" si="0"/>
         <v>239120.90000000002</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" t="str">
         <f>Ricavi!J19</f>
         <v>PCL2</v>
@@ -6727,11 +6843,11 @@
         <v>0.63902212980840634</v>
       </c>
       <c r="F18">
-        <f>D18*E18</f>
+        <f t="shared" si="0"/>
         <v>107563.4</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" t="str">
         <f>Ricavi!J20</f>
         <v>PCL3</v>
@@ -6749,11 +6865,11 @@
         <v>1.6503165205106214</v>
       </c>
       <c r="F19">
-        <f>D19*E19</f>
+        <f t="shared" si="0"/>
         <v>817690.5780000001</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" t="str">
         <f>Ricavi!J21</f>
         <v>PCL4</v>
@@ -6771,11 +6887,11 @@
         <v>2.6814489976240035</v>
       </c>
       <c r="F20">
-        <f>D20*E20</f>
+        <f t="shared" si="0"/>
         <v>1311384.0838799998</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" t="str">
         <f>Ricavi!J22</f>
         <v>PCL5</v>
@@ -6793,11 +6909,11 @@
         <v>2.25</v>
       </c>
       <c r="F21">
-        <f>D21*E21</f>
+        <f t="shared" si="0"/>
         <v>13860</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" t="str">
         <f>Ricavi!J23</f>
         <v>PF P1</v>
@@ -6815,11 +6931,17 @@
         <v>3.2527355771579307</v>
       </c>
       <c r="F22">
-        <f>D22*E22</f>
+        <f t="shared" si="0"/>
         <v>5593287</v>
       </c>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G22" t="s">
+        <v>205</v>
+      </c>
+      <c r="H22" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" t="str">
         <f>Ricavi!J24</f>
         <v>PF P2</v>
@@ -6837,11 +6959,14 @@
         <v>3.2730881131217542</v>
       </c>
       <c r="F23">
-        <f>D23*E23</f>
+        <f t="shared" si="0"/>
         <v>957375</v>
       </c>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G23" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" t="str">
         <f>Ricavi!J25</f>
         <v>PF P3</v>
@@ -6859,11 +6984,14 @@
         <v>3.2317332881662151</v>
       </c>
       <c r="F24">
-        <f>D24*E24</f>
+        <f t="shared" si="0"/>
         <v>1431011.5</v>
       </c>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G24" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" t="str">
         <f>Ricavi!J26</f>
         <v>PF P4</v>
@@ -6881,11 +7009,14 @@
         <v>3.1339358772483501</v>
       </c>
       <c r="F25">
-        <f>D25*E25</f>
+        <f t="shared" si="0"/>
         <v>25292348.015000001</v>
       </c>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G25" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" t="str">
         <f>Ricavi!J27</f>
         <v>PF P5</v>
@@ -6903,11 +7034,14 @@
         <v>0</v>
       </c>
       <c r="F26">
-        <f>D26*E26</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G26" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" t="str">
         <f>Ricavi!J28</f>
         <v>PF P6</v>
@@ -6925,11 +7059,14 @@
         <v>0</v>
       </c>
       <c r="F27">
-        <f>D27*E27</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G27" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" t="str">
         <f>Ricavi!J29</f>
         <v>PF P7</v>
@@ -6947,11 +7084,14 @@
         <v>0.96042054093345852</v>
       </c>
       <c r="F28">
-        <f>D28*E28</f>
+        <f t="shared" si="0"/>
         <v>634204.1</v>
       </c>
-    </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G28" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29" t="str">
         <f>Ricavi!J30</f>
         <v>PF V1</v>
@@ -6969,11 +7109,17 @@
         <v>1.4659810896505177</v>
       </c>
       <c r="F29">
-        <f>D29*E29</f>
+        <f t="shared" si="0"/>
         <v>747163.65</v>
       </c>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G29" t="s">
+        <v>206</v>
+      </c>
+      <c r="H29" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30" t="str">
         <f>Ricavi!J31</f>
         <v>PF V2</v>
@@ -6991,11 +7137,14 @@
         <v>1.5574062198816996</v>
       </c>
       <c r="F30">
-        <f>D30*E30</f>
+        <f t="shared" si="0"/>
         <v>3955786.879999999</v>
       </c>
-    </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G30" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B31" t="str">
         <f>Ricavi!J32</f>
         <v>PF V3</v>
@@ -7013,11 +7162,14 @@
         <v>1.5255310138943521</v>
       </c>
       <c r="F31">
-        <f>D31*E31</f>
+        <f t="shared" si="0"/>
         <v>1341915.05</v>
       </c>
-    </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G31" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B32" t="str">
         <f>Ricavi!J33</f>
         <v>PF V4</v>
@@ -7035,11 +7187,14 @@
         <v>1.5588271124689272</v>
       </c>
       <c r="F32">
-        <f>D32*E32</f>
+        <f t="shared" si="0"/>
         <v>903634.92999999993</v>
       </c>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G32" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B33" t="str">
         <f>Ricavi!J34</f>
         <v>PF V5</v>
@@ -7057,11 +7212,14 @@
         <v>1.4237468896798742</v>
       </c>
       <c r="F33">
-        <f>D33*E33</f>
+        <f t="shared" si="0"/>
         <v>637988.1</v>
       </c>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G33" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B34" t="str">
         <f>Ricavi!J35</f>
         <v>PF V6</v>
@@ -7079,11 +7237,14 @@
         <v>1.9231706379707918</v>
       </c>
       <c r="F34">
-        <f>D34*E34</f>
+        <f t="shared" si="0"/>
         <v>250204.5</v>
       </c>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G34" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B35" t="str">
         <f>Ricavi!J36</f>
         <v>PF V7</v>
@@ -7101,11 +7262,14 @@
         <v>1.1880509745127437</v>
       </c>
       <c r="F35">
-        <f>D35*E35</f>
+        <f t="shared" ref="F35:F66" si="1">D35*E35</f>
         <v>15848.6</v>
       </c>
-    </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G35" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B36" t="str">
         <f>Ricavi!J37</f>
         <v>PF V8</v>
@@ -7123,11 +7287,14 @@
         <v>1.6966731850403327</v>
       </c>
       <c r="F36">
-        <f>D36*E36</f>
+        <f t="shared" si="1"/>
         <v>138821.80000000002</v>
       </c>
-    </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G36" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B37" t="str">
         <f>Ricavi!J38</f>
         <v>PF V9</v>
@@ -7145,11 +7312,14 @@
         <v>1.6010133079847908</v>
       </c>
       <c r="F37">
-        <f>D37*E37</f>
+        <f t="shared" si="1"/>
         <v>33685.32</v>
       </c>
-    </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G37" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B38" t="str">
         <f>Ricavi!J39</f>
         <v>PF V10</v>
@@ -7167,11 +7337,14 @@
         <v>1.6058974358974358</v>
       </c>
       <c r="F38">
-        <f>D38*E38</f>
+        <f t="shared" si="1"/>
         <v>23486.25</v>
       </c>
-    </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G38" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B39" t="str">
         <f>Ricavi!J40</f>
         <v>PF V11</v>
@@ -7189,11 +7362,14 @@
         <v>0</v>
       </c>
       <c r="F39">
-        <f>D39*E39</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G39" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B40" t="str">
         <f>Ricavi!J41</f>
         <v>PF V12</v>
@@ -7211,11 +7387,14 @@
         <v>0</v>
       </c>
       <c r="F40">
-        <f>D40*E40</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G40" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B41" t="str">
         <f>Ricavi!J42</f>
         <v>PF V13</v>
@@ -7233,11 +7412,14 @@
         <v>0</v>
       </c>
       <c r="F41">
-        <f>D41*E41</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G41" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B42" t="str">
         <f>Ricavi!J43</f>
         <v>PF V14</v>
@@ -7255,11 +7437,14 @@
         <v>0</v>
       </c>
       <c r="F42">
-        <f>D42*E42</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G42" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B43" t="str">
         <f>Ricavi!J44</f>
         <v>PF V15</v>
@@ -7277,11 +7462,14 @@
         <v>2.1413333333333333</v>
       </c>
       <c r="F43">
-        <f>D43*E43</f>
+        <f t="shared" si="1"/>
         <v>64240</v>
       </c>
-    </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G43" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B44" t="str">
         <f>Ricavi!J45</f>
         <v>PF V16</v>
@@ -7299,11 +7487,14 @@
         <v>1.2007575757575757</v>
       </c>
       <c r="F44">
-        <f>D44*E44</f>
+        <f t="shared" si="1"/>
         <v>19812.5</v>
       </c>
-    </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G44" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B45" t="str">
         <f>Ricavi!J46</f>
         <v>PF A1</v>
@@ -7321,11 +7512,17 @@
         <v>1.2885862763813767</v>
       </c>
       <c r="F45">
-        <f>D45*E45</f>
+        <f t="shared" si="1"/>
         <v>121500.8</v>
       </c>
-    </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G45" t="s">
+        <v>207</v>
+      </c>
+      <c r="H45" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B46" t="str">
         <f>Ricavi!J47</f>
         <v>PF A2</v>
@@ -7343,11 +7540,14 @@
         <v>1.7877720617332806</v>
       </c>
       <c r="F46">
-        <f>D46*E46</f>
+        <f t="shared" si="1"/>
         <v>271062</v>
       </c>
-    </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G46" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B47" t="str">
         <f>Ricavi!J48</f>
         <v>PF A3</v>
@@ -7365,11 +7565,14 @@
         <v>1.8322972695210196</v>
       </c>
       <c r="F47">
-        <f>D47*E47</f>
+        <f t="shared" si="1"/>
         <v>754867.99680000008</v>
       </c>
-    </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G47" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B48" t="str">
         <f>Ricavi!J49</f>
         <v>PF A4</v>
@@ -7387,11 +7590,14 @@
         <v>0</v>
       </c>
       <c r="F48">
-        <f>D48*E48</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G48" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B49" t="str">
         <f>Ricavi!J50</f>
         <v>PF A5</v>
@@ -7409,11 +7615,14 @@
         <v>0</v>
       </c>
       <c r="F49">
-        <f>D49*E49</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G49" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B50" t="str">
         <f>Ricavi!J51</f>
         <v>PF A6</v>
@@ -7431,11 +7640,14 @@
         <v>0</v>
       </c>
       <c r="F50">
-        <f>D50*E50</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G50" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B51" t="str">
         <f>Ricavi!J52</f>
         <v>PF A7</v>
@@ -7453,11 +7665,14 @@
         <v>1.6397767269078427</v>
       </c>
       <c r="F51">
-        <f>D51*E51</f>
+        <f t="shared" si="1"/>
         <v>4624923.0109999999</v>
       </c>
-    </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G51" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B52" t="str">
         <f>Ricavi!J53</f>
         <v>PF A8</v>
@@ -7475,11 +7690,14 @@
         <v>1.6271923465786613</v>
       </c>
       <c r="F52">
-        <f>D52*E52</f>
+        <f t="shared" si="1"/>
         <v>255897.15000000002</v>
       </c>
-    </row>
-    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G52" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B53" t="str">
         <f>Ricavi!J54</f>
         <v>PF A9</v>
@@ -7497,11 +7715,14 @@
         <v>1.5522070782270072</v>
       </c>
       <c r="F53">
-        <f>D53*E53</f>
+        <f t="shared" si="1"/>
         <v>406569.6</v>
       </c>
-    </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G53" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B54" t="str">
         <f>Ricavi!J55</f>
         <v>PF A10</v>
@@ -7519,11 +7740,14 @@
         <v>1.2455093073420147</v>
       </c>
       <c r="F54">
-        <f>D54*E54</f>
+        <f t="shared" si="1"/>
         <v>623601.6</v>
       </c>
-    </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G54" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B55" t="str">
         <f>Ricavi!J56</f>
         <v>PF A11</v>
@@ -7541,11 +7765,14 @@
         <v>1.9325902603525706</v>
       </c>
       <c r="F55">
-        <f>D55*E55</f>
+        <f t="shared" si="1"/>
         <v>120920.23999999999</v>
       </c>
-    </row>
-    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G55" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B56" t="str">
         <f>Ricavi!J57</f>
         <v>PF A12</v>
@@ -7563,11 +7790,14 @@
         <v>2.009165683120187</v>
       </c>
       <c r="F56">
-        <f>D56*E56</f>
+        <f t="shared" si="1"/>
         <v>1864033.6000000003</v>
       </c>
-    </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G56" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B57" t="str">
         <f>Ricavi!J58</f>
         <v>PF A13</v>
@@ -7585,11 +7815,14 @@
         <v>1.6307046552057176</v>
       </c>
       <c r="F57">
-        <f>D57*E57</f>
+        <f t="shared" si="1"/>
         <v>211053.95</v>
       </c>
-    </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G57" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B58" t="str">
         <f>Ricavi!J59</f>
         <v>PF A14</v>
@@ -7607,11 +7840,14 @@
         <v>1.9791817665113107</v>
       </c>
       <c r="F58">
-        <f>D58*E58</f>
+        <f t="shared" si="1"/>
         <v>261162.93</v>
       </c>
-    </row>
-    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G58" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B59" t="str">
         <f>Ricavi!J60</f>
         <v>PF A15</v>
@@ -7629,11 +7865,14 @@
         <v>1.7865580217289871</v>
       </c>
       <c r="F59">
-        <f>D59*E59</f>
+        <f t="shared" si="1"/>
         <v>670093.24999999988</v>
       </c>
-    </row>
-    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G59" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B60" t="str">
         <f>Ricavi!J61</f>
         <v>PF A16</v>
@@ -7651,11 +7890,14 @@
         <v>1.6128909403745617</v>
       </c>
       <c r="F60">
-        <f>D60*E60</f>
+        <f t="shared" si="1"/>
         <v>243723.95</v>
       </c>
-    </row>
-    <row r="61" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G60" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B61" t="str">
         <f>Ricavi!J62</f>
         <v>PF A17</v>
@@ -7673,11 +7915,14 @@
         <v>1.9365259652409199</v>
       </c>
       <c r="F61">
-        <f>D61*E61</f>
+        <f t="shared" si="1"/>
         <v>465201.95</v>
       </c>
-    </row>
-    <row r="62" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G61" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B62" t="str">
         <f>Ricavi!J63</f>
         <v>PF A18</v>
@@ -7695,11 +7940,14 @@
         <v>1.0338126145387905</v>
       </c>
       <c r="F62">
-        <f>D62*E62</f>
+        <f t="shared" si="1"/>
         <v>406164.3</v>
       </c>
-    </row>
-    <row r="63" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G62" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B63" t="str">
         <f>Ricavi!J64</f>
         <v>PF A19</v>
@@ -7717,11 +7965,14 @@
         <v>1.59928712602404</v>
       </c>
       <c r="F63">
-        <f>D63*E63</f>
+        <f t="shared" si="1"/>
         <v>2120046.9999999879</v>
       </c>
-    </row>
-    <row r="64" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G63" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="64" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B64" t="str">
         <f>Ricavi!J65</f>
         <v>Spese trasporto</v>
@@ -7738,15 +7989,15 @@
         <v>1</v>
       </c>
       <c r="F64">
-        <f>D64*E64</f>
+        <f t="shared" si="1"/>
         <v>25000</v>
       </c>
-      <c r="G64" t="str">
+      <c r="H64" t="str">
         <f>"Riaccredito trasporti"</f>
         <v>Riaccredito trasporti</v>
       </c>
     </row>
-    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B65" t="str">
         <f>Ricavi!J66</f>
         <v>Premio Year22</v>
@@ -7767,16 +8018,16 @@
         <f>-D65*E65</f>
         <v>-227771.84999999998</v>
       </c>
-      <c r="G65" t="str">
+      <c r="H65" t="str">
         <f>"Premio clienti (ricavo negativo)"</f>
         <v>Premio clienti (ricavo negativo)</v>
       </c>
     </row>
-    <row r="67" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="E67" s="104" t="s">
+    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E67" s="93" t="s">
         <v>200</v>
       </c>
-      <c r="F67" s="104">
+      <c r="F67" s="93">
         <f>SUM(F3:F65)</f>
         <v>57945067.876579978</v>
       </c>
@@ -7807,22 +8058,22 @@
   <sheetData>
     <row r="1" spans="2:16" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="101" t="s">
+      <c r="B2" s="102" t="s">
         <v>134</v>
       </c>
-      <c r="C2" s="102"/>
-      <c r="D2" s="102"/>
-      <c r="E2" s="102"/>
-      <c r="F2" s="102"/>
-      <c r="G2" s="102"/>
-      <c r="H2" s="102"/>
-      <c r="I2" s="102"/>
-      <c r="J2" s="102"/>
-      <c r="K2" s="102"/>
-      <c r="L2" s="102"/>
-      <c r="M2" s="102"/>
-      <c r="N2" s="102"/>
-      <c r="O2" s="103"/>
+      <c r="C2" s="103"/>
+      <c r="D2" s="103"/>
+      <c r="E2" s="103"/>
+      <c r="F2" s="103"/>
+      <c r="G2" s="103"/>
+      <c r="H2" s="103"/>
+      <c r="I2" s="103"/>
+      <c r="J2" s="103"/>
+      <c r="K2" s="103"/>
+      <c r="L2" s="103"/>
+      <c r="M2" s="103"/>
+      <c r="N2" s="103"/>
+      <c r="O2" s="104"/>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B3" s="12" t="s">
@@ -8181,6 +8432,263 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EB61E9C-EC3D-49DF-83B5-89D531594792}">
+  <dimension ref="B2:H18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection sqref="A1:I19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="58.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>216</v>
+      </c>
+      <c r="C2">
+        <v>3450000</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>217</v>
+      </c>
+      <c r="C3">
+        <v>0.41</v>
+      </c>
+      <c r="E3" t="s">
+        <v>201</v>
+      </c>
+      <c r="F3" t="s">
+        <v>214</v>
+      </c>
+      <c r="G3" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>218</v>
+      </c>
+      <c r="C4">
+        <f>1-C3</f>
+        <v>0.59000000000000008</v>
+      </c>
+      <c r="E4" t="s">
+        <v>113</v>
+      </c>
+      <c r="F4">
+        <f>SUMIF(RicaviBudget!$G:$G,"P",RicaviBudget!$D:$D)</f>
+        <v>14624683</v>
+      </c>
+      <c r="G4">
+        <f>F4/1000</f>
+        <v>14624.683000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>219</v>
+      </c>
+      <c r="C5">
+        <v>8997222.2200000007</v>
+      </c>
+      <c r="E5" t="s">
+        <v>211</v>
+      </c>
+      <c r="F5">
+        <f>SUMIF(RicaviBudget!$G:$G,"V",RicaviBudget!$D:$D)</f>
+        <v>6470002</v>
+      </c>
+      <c r="G5">
+        <f t="shared" ref="G5:G6" si="0">F5/1000</f>
+        <v>6470.0020000000004</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>220</v>
+      </c>
+      <c r="C6">
+        <v>4300000</v>
+      </c>
+      <c r="E6" t="s">
+        <v>212</v>
+      </c>
+      <c r="F6">
+        <f>SUMIF(RicaviBudget!$G:$G,"A",RicaviBudget!$D:$CD)</f>
+        <v>9655208.9900000002</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>9655.208990000001</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>213</v>
+      </c>
+      <c r="F7">
+        <f xml:space="preserve"> SUM(F4:F6)</f>
+        <v>30749893.990000002</v>
+      </c>
+      <c r="G7">
+        <f>G6+G5+G4</f>
+        <v>30749.893990000004</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>221</v>
+      </c>
+      <c r="C8">
+        <f>C2*C3</f>
+        <v>1414500</v>
+      </c>
+      <c r="F8" t="s">
+        <v>199</v>
+      </c>
+      <c r="G8" t="s">
+        <v>203</v>
+      </c>
+      <c r="H8" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>222</v>
+      </c>
+      <c r="C9">
+        <f>C2*C4</f>
+        <v>2035500.0000000002</v>
+      </c>
+      <c r="F9" t="s">
+        <v>231</v>
+      </c>
+      <c r="G9">
+        <f>(G6*0.93+G5*0.64)*C18</f>
+        <v>7080.2103150872417</v>
+      </c>
+      <c r="H9" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F10" t="s">
+        <v>232</v>
+      </c>
+      <c r="G10">
+        <f xml:space="preserve"> ( G4*140 + G5*60 + G6*65 + 3300000 ) * C17</f>
+        <v>1110442.5180509007</v>
+      </c>
+      <c r="H10" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>223</v>
+      </c>
+      <c r="C11">
+        <f>C8/C5</f>
+        <v>0.15721518991224825</v>
+      </c>
+      <c r="F11" t="s">
+        <v>233</v>
+      </c>
+      <c r="G11">
+        <f>-'CE 21-22'!F15 *1.025</f>
+        <v>153750</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>224</v>
+      </c>
+      <c r="C12">
+        <f>C9/C6</f>
+        <v>0.47337209302325589</v>
+      </c>
+      <c r="F12" t="s">
+        <v>234</v>
+      </c>
+      <c r="G12">
+        <f>G7*10.24</f>
+        <v>314878.91445760004</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F13" t="s">
+        <v>235</v>
+      </c>
+      <c r="G13">
+        <f>G7*43.2</f>
+        <v>1328395.4203680002</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>225</v>
+      </c>
+      <c r="C14">
+        <v>0.11</v>
+      </c>
+      <c r="F14" t="s">
+        <v>236</v>
+      </c>
+      <c r="G14">
+        <f>(SUMIF(RicaviBudget!$G:$G,"P",RicaviBudget!$F:$F)+SUMIF(RicaviBudget!$G:$G,"V",RicaviBudget!$F:$F))*0.02</f>
+        <v>840816.26390000002</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>226</v>
+      </c>
+      <c r="C15">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F15" t="s">
+        <v>237</v>
+      </c>
+      <c r="G15">
+        <f>SUM(G9:G14)</f>
+        <v>3755363.3270915882</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>227</v>
+      </c>
+      <c r="C17">
+        <f>C11*(1+C14)</f>
+        <v>0.17450886080259559</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>228</v>
+      </c>
+      <c r="C18">
+        <f>C12*(1+C15)</f>
+        <v>0.53964418604651176</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1DC2D69-4CDB-4944-95A7-150A65922A87}">
   <dimension ref="B1:B28"/>
   <sheetViews>
@@ -8321,7 +8829,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BC74C4D-8FA0-4227-922B-636E2D04E620}">
   <dimension ref="B1:I28"/>
   <sheetViews>

</xml_diff>

<commit_message>
aggiunta del foglio di calcolo FixedCostsBudget
</commit_message>
<xml_diff>
--- a/Progetto_sdg.xlsx
+++ b/Progetto_sdg.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marco\Documents\GitHub\script-analisi-scostamenti\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C590D7E-DD1F-4900-B8C4-93081D601457}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B8E4B70-73E2-412A-B5B3-D44B6D1BB94B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CE 21-22" sheetId="3" r:id="rId1"/>
@@ -19,10 +19,11 @@
     <sheet name="VariableCosts" sheetId="4" r:id="rId4"/>
     <sheet name="VariableCostsBudget" sheetId="8" r:id="rId5"/>
     <sheet name="FixedCosts" sheetId="5" r:id="rId6"/>
-    <sheet name="Others" sheetId="6" r:id="rId7"/>
+    <sheet name="FixedCostsBudget" sheetId="9" r:id="rId7"/>
+    <sheet name="Others" sheetId="6" r:id="rId8"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId8"/>
+    <externalReference r:id="rId9"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="255">
   <si>
     <t>MP1</t>
   </si>
@@ -849,6 +850,42 @@
   <si>
     <t>costo CO2</t>
   </si>
+  <si>
+    <t xml:space="preserve">Costo del personale </t>
+  </si>
+  <si>
+    <t>Manutenzioni</t>
+  </si>
+  <si>
+    <t>Altri oneri del personale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assicurazioni </t>
+  </si>
+  <si>
+    <t>Consulenze tecniche e canoni acque</t>
+  </si>
+  <si>
+    <t>Costo per godimento di beni di terzi</t>
+  </si>
+  <si>
+    <t>Consulenze e amministrazioni</t>
+  </si>
+  <si>
+    <t>Spese ufficio varie e oneri diversi di gestione</t>
+  </si>
+  <si>
+    <t>Imposte e tasse varie non sul reddito</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Totale budget costi fissi di produzione </t>
+  </si>
+  <si>
+    <t>Totale budget costi struttura comm./amm.va</t>
+  </si>
+  <si>
+    <t>TOTALE BUDGET COSTI FISSI</t>
+  </si>
 </sst>
 </file>
 
@@ -868,7 +905,7 @@
     <numFmt numFmtId="172" formatCode="_-&quot;L.&quot;\ * #,##0_-;\-&quot;L.&quot;\ * #,##0_-;_-&quot;L.&quot;\ * &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="173" formatCode="_-[$€-2]\ * #,##0.00_-;\-[$€-2]\ * #,##0.00_-;_-[$€-2]\ * &quot;-&quot;??_-"/>
   </numFmts>
-  <fonts count="27" x14ac:knownFonts="1">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1056,6 +1093,12 @@
       <name val="Calibri Light"/>
       <family val="2"/>
       <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="13">
@@ -1529,7 +1572,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -1762,6 +1805,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="27" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -2677,7 +2723,7 @@
   <dimension ref="B1:J62"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="92" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3364,8 +3410,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:XFD1048576"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+    <sheetView showGridLines="0" topLeftCell="A51" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6473,7 +6519,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EAEFA6D-2B43-44D4-9785-BA525C9ED11E}">
   <dimension ref="B2:H67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A43" workbookViewId="0">
       <selection activeCell="H45" sqref="H45"/>
     </sheetView>
   </sheetViews>
@@ -8450,7 +8496,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EB61E9C-EC3D-49DF-83B5-89D531594792}">
   <dimension ref="B2:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
@@ -8751,7 +8797,7 @@
   <dimension ref="B1:B28"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8888,6 +8934,133 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92EB1E3B-0C1C-4993-9177-FBCEDBD20284}">
+  <dimension ref="B2:C26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:C26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="41.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>243</v>
+      </c>
+      <c r="C2">
+        <f>-'CE 21-22'!F22+50*12*100</f>
+        <v>5570785.9100000001</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>244</v>
+      </c>
+      <c r="C4">
+        <f>-'CE 21-22'!F23-150000</f>
+        <v>1050000</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>245</v>
+      </c>
+      <c r="C6">
+        <f>-'CE 21-22'!F24*1.025</f>
+        <v>307500</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>246</v>
+      </c>
+      <c r="C8">
+        <f>-'CE 21-22'!F25*1.025</f>
+        <v>151700</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>247</v>
+      </c>
+      <c r="C10">
+        <f>-'CE 21-22'!F26*1.025</f>
+        <v>309550</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>248</v>
+      </c>
+      <c r="C12">
+        <f>-'CE 21-22'!F27*1.025</f>
+        <v>212174.99999999997</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B14" s="93" t="s">
+        <v>252</v>
+      </c>
+      <c r="C14" s="93">
+        <f>SUM(C12+C10+C8+C6+C4+C2)</f>
+        <v>7601710.9100000001</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>249</v>
+      </c>
+      <c r="C17">
+        <f>-'CE 21-22'!F29*1.025</f>
+        <v>563750</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="105" t="s">
+        <v>250</v>
+      </c>
+      <c r="C19">
+        <f>-'CE 21-22'!F30*1.025</f>
+        <v>307500</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>251</v>
+      </c>
+      <c r="C21">
+        <f>-'CE 21-22'!F31*1.025</f>
+        <v>102499.99999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="93" t="s">
+        <v>253</v>
+      </c>
+      <c r="C23" s="93">
+        <f>SUM(C17+C19+C21)</f>
+        <v>973750</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26" s="93" t="s">
+        <v>254</v>
+      </c>
+      <c r="C26" s="93">
+        <f>SUM(C23+C14)</f>
+        <v>8575460.9100000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BC74C4D-8FA0-4227-922B-636E2D04E620}">
   <dimension ref="B1:I28"/>
   <sheetViews>

</xml_diff>

<commit_message>
aggiunta commenti ai budget
aggiunta di note ad alcune celle e controllo eventuali errori
</commit_message>
<xml_diff>
--- a/Progetto_sdg.xlsx
+++ b/Progetto_sdg.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utente\Desktop\Nicola\UNIBG\Sistemi di controllo di gestione\script analisi scostamenti\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Celeste\Documents\GitHub\script-analisi-scostamenti\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{028201B4-78A2-4FF7-B7F9-4B183C648530}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85D645E8-41BE-4157-8392-688F71BDFA4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="675" firstSheet="5" activeTab="9" xr2:uid="{47D82A9E-1214-4F6E-A405-C3A19453CBD3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="675" firstSheet="4" activeTab="8" xr2:uid="{47D82A9E-1214-4F6E-A405-C3A19453CBD3}"/>
   </bookViews>
   <sheets>
     <sheet name="CE 21-22" sheetId="3" r:id="rId1"/>
@@ -45,6 +45,1695 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Celeste</author>
+  </authors>
+  <commentList>
+    <comment ref="O3" authorId="0" shapeId="0" xr:uid="{10CAA52E-B4AB-44AF-954C-8F9ADEFB794A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Celeste:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+aggiunta dazio per alcuni prodotti importati</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J4" authorId="0" shapeId="0" xr:uid="{E1204172-960F-49A5-8FE8-1F7A146C50BD}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Celeste:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+materia prima</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J18" authorId="0" shapeId="0" xr:uid="{7D5002F4-B2EA-4CFF-89CD-CE73B7448870}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Celeste:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+prodotto conto lavorazione</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J23" authorId="0" shapeId="0" xr:uid="{28B5F12F-C0A9-4450-A5B2-5308824BE9DC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Celeste:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+prodotti finiti
+3 tipologie
+- A acriliche (emulsioni)
+- V viniliche (emulsioni)
+- P polveri (non emulsioni)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J66" authorId="0" shapeId="0" xr:uid="{45973941-ABC1-4C3E-AFFD-519015266110}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Celeste:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+ricavo negativo</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Celeste</author>
+  </authors>
+  <commentList>
+    <comment ref="E2" authorId="0" shapeId="0" xr:uid="{CBB31D9D-3173-4381-BF3B-3D46A53F6751}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Celeste:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+prezzo di vendita prodotto</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F2" authorId="0" shapeId="0" xr:uid="{01140BF7-5F8E-4307-BC93-349DFF22BC14}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Celeste:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+costo medio per pezzo in euro al Kg</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Celeste</author>
+  </authors>
+  <commentList>
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{FEED04D6-90BE-440D-B3E2-D037356569C0}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Celeste:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+% elettricità su enegia totale 2021</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H3" authorId="0" shapeId="0" xr:uid="{42F60721-A89D-459E-9A7D-1B952B699EE7}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Celeste:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+formula che si può dividere in due:
+1) calcolo totale tonn di vapore usate per un prodotto
+2) moltiplico il risultato con gli smc di metano per tonn di vapore</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{5D955DEE-E91D-4ACD-8E0A-9DA1EFFEBEAF}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Celeste:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+% metano su enegia totale 2021</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I4" authorId="0" shapeId="0" xr:uid="{17EEE312-7932-4FC1-B957-556D67D428E1}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Celeste:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+è una somma, tra l'energia usata per produrre polveri e l'energia usata per produrre le viniliche usate poi per le polveri</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{FDC56793-B754-4B4B-93EA-A59D27E49E32}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Celeste:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+elettricità utilizzata 2021</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B6" authorId="0" shapeId="0" xr:uid="{9E1683E2-9775-40A6-997D-2F4C30A2A4E0}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Celeste:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+metri cubi di metano usati nel 2021</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E6" authorId="0" shapeId="0" xr:uid="{570A9678-407A-454C-B63C-625B612EF7B1}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Celeste:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+come da nota [i], i prodotti di conto lavoro sono processati nel reparto acriliche (per tutti i prodotti produzione=vendite)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B8" authorId="0" shapeId="0" xr:uid="{89C2E11A-CAE9-444E-A492-09D59EBAC144}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Celeste:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+calolo energia dedicata a elettricità</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{E045043C-C6A2-48FE-9A78-6B46220C2E1D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Celeste:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+calolo energia dedicata a metano</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F9" authorId="0" shapeId="0" xr:uid="{4942943F-CDB2-40E8-B4F9-F35FAB4FAF53}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Celeste:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+costo previsto del metano per il 2022</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F10" authorId="0" shapeId="0" xr:uid="{1F9EA29B-2277-487A-B2FF-D015FD262896}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Celeste:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+costo previsto per elettricità per il 2022</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B11" authorId="0" shapeId="0" xr:uid="{944C56EB-F0E9-4BE9-B107-DBA1159EBD21}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Celeste:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+costo per ogni kWh 2021</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F11" authorId="0" shapeId="0" xr:uid="{DF2DD38E-BE88-46E8-9F6B-66827F29CC0E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Celeste:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+aumento previsto del 2.5%</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B12" authorId="0" shapeId="0" xr:uid="{91597BBA-2CC7-488C-AAA6-8084DFA04E17}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Celeste:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+costo per ogni smc di metano 2021</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F12" authorId="0" shapeId="0" xr:uid="{10AD7644-2E75-4ACD-8CC7-870B3FC074A0}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Celeste:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+si considerano anche le polveri perché le viniliche che usano producono emulsioni</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F13" authorId="0" shapeId="0" xr:uid="{B067C4AE-F6B7-4F88-AE59-E8747A6C4005}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Celeste:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+costo previsto per trasporti per il 2022</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B14" authorId="0" shapeId="0" xr:uid="{F20D4AE2-20E0-4B64-B33F-4D4ECBF6C790}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Celeste:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+% incremento rispetto a valore in bilancio (costo elettricità 2021)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F14" authorId="0" shapeId="0" xr:uid="{C3112D41-D453-46B3-95DF-8FC9C0895C4E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Celeste:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+costi aggiuntivi per polveri per il 2022</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B15" authorId="0" shapeId="0" xr:uid="{2A61C2C3-FB80-43F6-8615-99F3A8FA70B4}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Celeste:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+% incremento rispetto a valore in bilancio (costo Metano 2021)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F15" authorId="0" shapeId="0" xr:uid="{E1033EB4-6399-4A00-B171-1382E93DF77E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Celeste:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+costo delle quote CO2 previste per 2022</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B17" authorId="0" shapeId="0" xr:uid="{75008C81-DEF1-4322-B6E6-B4120072C5D9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Celeste:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+nuovo prezzo previsto per un kWh</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B18" authorId="0" shapeId="0" xr:uid="{B5F38932-F554-4078-907A-7C2CEEC3DD01}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Celeste:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+nuovo prezzo previsto per un smc di metano</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B20" authorId="0" shapeId="0" xr:uid="{583BEE5F-4D9C-4A72-9431-475A31AEF102}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Celeste:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+tonn di vapore per produrre una tonn di acriliche</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B21" authorId="0" shapeId="0" xr:uid="{862EFE1E-7EB7-4E50-ADEB-B1DF53532BDA}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Celeste:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+tonn di vapore per produrre una tonn di viniliche</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B22" authorId="0" shapeId="0" xr:uid="{5EE4EF53-E133-4CA6-AFD8-5BAD8F177B02}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Celeste:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+servono produrre 1.67tonn di emulsioni di viniliche per produrre 1tonn di polveri</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B23" authorId="0" shapeId="0" xr:uid="{BC9729FA-5AC1-4B44-985C-09CFF8511863}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Celeste:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+tonn di vapore per produrre una tonn di polveri. 
+Il vapore qui è usato solamente per le 1.67tonn di viniliche</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B24" authorId="0" shapeId="0" xr:uid="{D3741848-4A19-4F51-ADE2-C3D6A24F16EC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Celeste:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+consumo di metano per ogni tonn di vapore</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B26" authorId="0" shapeId="0" xr:uid="{F195D654-4E0B-40D5-A16B-7608A557207E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Celeste:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+elettricità usata per produrre una tonn di polveri (ancora non si considera quella per produrre le viniliche usate dalle polveri)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B27" authorId="0" shapeId="0" xr:uid="{D02E10BC-0551-4BE8-A005-C111BA8152AE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Celeste:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+elettricità usata per produrre una tonn di viniliche</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B28" authorId="0" shapeId="0" xr:uid="{73C40828-7D9F-4E7C-9A64-C79ADAC8F772}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Celeste:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+elettricità usata per produrre una tonn di acriliche</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B30" authorId="0" shapeId="0" xr:uid="{336C4CAD-DBEE-4F3F-980B-5812C0526FEA}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Celeste:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+costi annuali elettricità per servizi non dedicati alla produzione</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B32" authorId="0" shapeId="0" xr:uid="{E1EC3A12-E92B-46BA-8458-74C72EB867CE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Celeste:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+il costo è solo sulle emulsioni, le polveri non le producono</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B34" authorId="0" shapeId="0" xr:uid="{A9D594D5-D77A-4F84-8A91-0B22FCD6BC8B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Celeste:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+valore a bilancio sul costo medio di trasporto di una tonn di prodotto</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B35" authorId="0" shapeId="0" xr:uid="{BAFD87A7-0EAD-49C9-B498-D44633E6D9A6}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Celeste:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+% aumento costi previsto nei trasporti</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B36" authorId="0" shapeId="0" xr:uid="{6200E078-49AD-4FA4-9936-4CEF5563C9DF}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Celeste:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+valore previsto costi trasporto 2022</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B38" authorId="0" shapeId="0" xr:uid="{A74F445A-77B3-4F81-97ED-7EAF12530F7E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Celeste:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+sarebbero le commissioni di vendita, per ogni polvere venduta c'è un costo aggiuntivo del 2%</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B40" authorId="0" shapeId="0" xr:uid="{B0E9ACB3-D379-4D37-9120-AB5488FACE9E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Celeste:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+totale tonn di vapore prodotte per polveri previste per 2022</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B41" authorId="0" shapeId="0" xr:uid="{5CB65CC2-54EB-4CBC-959D-79A3F384E2EB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Celeste:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+totale tonn di vapore prodotte per viniliche previste per 2022</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B42" authorId="0" shapeId="0" xr:uid="{6824BFF4-6B71-4347-9866-20609EF70062}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Celeste:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+totale tonn di vapore prodotte per acriliche previste per 2022</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B44" authorId="0" shapeId="0" xr:uid="{5579F39C-ACCB-427E-9AFF-E68D60B845ED}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Celeste:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+quote di CO2 da pagare (25% di quelle usate)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B45" authorId="0" shapeId="0" xr:uid="{AB501C90-61B0-4375-8751-6EC9ED7246F5}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Celeste:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+costo di una quota CO2 per ogni tonn di vapore prodotta</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Celeste</author>
+  </authors>
+  <commentList>
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{5A515C47-0D77-4945-928D-3B54802E0BEA}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Celeste:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+preso il valore a bilancio 2021 come da note si aggiunge una spesa di 50euro per 100 persone ogni mese</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{5A134A16-68F1-4F3F-932A-480CCD054680}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Celeste:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+previsto valore a ribasso di 150k rispetto a 2021</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{467A9F08-D997-4163-9738-8ED546CAC2AB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Celeste:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+aumento del 2.5% per prudenza</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{1AA983D4-E67F-472F-9B27-2C34DA3EDD9A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Celeste:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+aumento del 2.5% per prudenza</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B11" authorId="0" shapeId="0" xr:uid="{B9511280-BD05-447E-8142-86F1D99BF07F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Celeste:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+aumento del 2.5% per prudenza</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B13" authorId="0" shapeId="0" xr:uid="{4A1C1C79-FC40-4009-8127-97C5D3C17B7C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Celeste:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+aumento del 2.5% per prudenza</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B15" authorId="0" shapeId="0" xr:uid="{15713A8D-1872-4821-8C52-5C0F117816C4}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Celeste:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+sono i costi fissi correlati strettamente alle attività di produzione</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B18" authorId="0" shapeId="0" xr:uid="{2CC72DBE-36AD-4DD8-B868-DDC18B61A7D7}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Celeste:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+aumento del 2.5% per prudenza</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B20" authorId="0" shapeId="0" xr:uid="{9FE0E382-FABA-4515-880B-FE949A6011BF}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Celeste:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+aumento del 2.5% per prudenza</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B22" authorId="0" shapeId="0" xr:uid="{600B6554-2959-4C17-B1EF-7625F79BC02A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Celeste:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+aumento del 2.5% per prudenza</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B24" authorId="0" shapeId="0" xr:uid="{673815C0-95D5-4379-934B-DB231699DA31}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Celeste:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+sono i costi fissi per servizi generali esterni</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Celeste</author>
+  </authors>
+  <commentList>
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{B0AD8B6B-8B8D-46F1-B778-89D9559CB3F0}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Celeste:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+in linea con 2021</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{80772B30-D2F2-458C-8863-C25956F8EB64}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Celeste:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+aggiunto al valore a bilancio nel 2021 la quota del primo anno per il nuovo investimento</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{46E3E794-D0A7-43A7-83C8-D68040445650}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Celeste:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Non sono previste svalutazioni credito</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{C1D1BEBD-2FCD-416E-B0B8-DD3B4F0562F7}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Celeste:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+nuova linea di credito con inizio previsto a giugno 2022  </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B11" authorId="0" shapeId="0" xr:uid="{5053B4BF-1C3C-4BFF-B454-33C928BA30CB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Celeste:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Non sono previsti proventi finanziari</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B13" authorId="0" shapeId="0" xr:uid="{248F359D-CA46-4B66-BF09-D5DC47D8449B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Celeste:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Non sono previsti oneri straordinari</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B15" authorId="0" shapeId="0" xr:uid="{D550298A-A392-4F19-BC1C-23FFDF7479C5}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Celeste:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Non sono previsti proventi straordinari</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B17" authorId="0" shapeId="0" xr:uid="{1989D6F5-1999-4AED-96AD-328E0286D822}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Celeste:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Non sono previsto svalutazioni e/o accantonamenti</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B19" authorId="0" shapeId="0" xr:uid="{6805CA83-6890-4F94-BCB1-6A825B74DA67}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Celeste:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+30% del risultato ante imposte</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
@@ -979,9 +2668,6 @@
     <t>cons smc per ton P (comprese le v)</t>
   </si>
   <si>
-    <t>nuovo investimento</t>
-  </si>
-  <si>
     <t>quota primo anno</t>
   </si>
   <si>
@@ -1376,6 +3062,9 @@
   </si>
   <si>
     <t>Sooma ∆ Verifica</t>
+  </si>
+  <si>
+    <t>nuovo investimento (imm materiali)</t>
   </si>
 </sst>
 </file>
@@ -1402,7 +3091,7 @@
     <numFmt numFmtId="178" formatCode="#,##0.00_ ;[Red]\-#,##0.00\ "/>
     <numFmt numFmtId="179" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="33" x14ac:knownFonts="1">
+  <fonts count="35" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1634,6 +3323,19 @@
       <name val="Calibri Light"/>
       <family val="2"/>
       <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="21">
@@ -2179,7 +3881,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="159">
+  <cellXfs count="158">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -2518,7 +4220,6 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="19">
     <cellStyle name="Euro" xfId="16" xr:uid="{6609C029-AE67-4DF2-BB38-0E304B6F97A8}"/>
@@ -3432,8 +5133,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C09E9022-8714-451A-AC8C-ADBBD3500E3D}">
   <dimension ref="B1:N62"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="91" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView topLeftCell="A12" zoomScale="91" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3558,7 +5259,7 @@
       <c r="E11" s="44"/>
       <c r="F11" s="45"/>
       <c r="J11" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.3">
@@ -3574,17 +5275,17 @@
         <v>1</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="M12" s="98">
         <f xml:space="preserve"> 1.17</f>
         <v>1.17</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.3">
@@ -3601,17 +5302,17 @@
         <v>1</v>
       </c>
       <c r="K13" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="L13" s="1" t="s">
         <v>282</v>
-      </c>
-      <c r="L13" s="1" t="s">
-        <v>283</v>
       </c>
       <c r="M13" s="1">
         <f>J13/M12</f>
         <v>0.85470085470085477</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.3">
@@ -3630,7 +5331,7 @@
       </c>
       <c r="G14" s="2"/>
       <c r="M14" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.3">
@@ -4151,8 +5852,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBC2357A-B255-476A-B362-53609C625BCC}">
   <dimension ref="A2:L142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A86" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="E107" sqref="E107"/>
+    <sheetView zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4171,7 +5872,7 @@
   <sheetData>
     <row r="2" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B2" s="156" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C2" s="156"/>
       <c r="D2" s="156"/>
@@ -4180,16 +5881,16 @@
         <v>124</v>
       </c>
       <c r="G2" s="115" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="H2" s="134" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="I2" t="s">
+        <v>389</v>
+      </c>
+      <c r="J2" t="s">
         <v>390</v>
-      </c>
-      <c r="J2" t="s">
-        <v>391</v>
       </c>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.3">
@@ -4197,10 +5898,10 @@
         <v>124</v>
       </c>
       <c r="C3" s="112" t="s">
+        <v>304</v>
+      </c>
+      <c r="D3" s="112" t="s">
         <v>305</v>
-      </c>
-      <c r="D3" s="112" t="s">
-        <v>306</v>
       </c>
       <c r="E3" s="115"/>
       <c r="F3" s="115" t="s">
@@ -4377,7 +6078,7 @@
       <c r="D9" s="157"/>
       <c r="E9" s="131"/>
       <c r="F9" s="134" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="G9" s="138">
         <f>SUM(G3:G7)</f>
@@ -4474,7 +6175,7 @@
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C16" s="132">
         <f>SUM(C4:C8)</f>
@@ -4491,7 +6192,7 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B18" s="115" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C18" s="140">
         <f>SUM(C10:C14)</f>
@@ -4501,45 +6202,45 @@
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="115"/>
       <c r="B20" s="116" t="s">
+        <v>306</v>
+      </c>
+      <c r="C20" s="116" t="s">
         <v>307</v>
       </c>
-      <c r="C20" s="116" t="s">
+      <c r="D20" s="116" t="s">
         <v>308</v>
       </c>
-      <c r="D20" s="116" t="s">
+      <c r="E20" s="116" t="s">
         <v>309</v>
       </c>
-      <c r="E20" s="116" t="s">
+      <c r="F20" s="116" t="s">
         <v>310</v>
       </c>
-      <c r="F20" s="116" t="s">
+      <c r="G20" s="116" t="s">
+        <v>406</v>
+      </c>
+      <c r="H20" s="116" t="s">
         <v>311</v>
       </c>
-      <c r="G20" s="116" t="s">
+      <c r="I20" s="116" t="s">
+        <v>405</v>
+      </c>
+      <c r="J20" s="116" t="s">
         <v>407</v>
       </c>
-      <c r="H20" s="116" t="s">
-        <v>312</v>
-      </c>
-      <c r="I20" s="116" t="s">
-        <v>406</v>
-      </c>
-      <c r="J20" s="116" t="s">
+      <c r="K20" s="116" t="s">
         <v>408</v>
       </c>
-      <c r="K20" s="116" t="s">
-        <v>409</v>
-      </c>
       <c r="L20" s="116" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="155" t="s">
+        <v>312</v>
+      </c>
+      <c r="B21" s="117" t="s">
         <v>313</v>
-      </c>
-      <c r="B21" s="117" t="s">
-        <v>314</v>
       </c>
       <c r="C21" s="118">
         <f>C4</f>
@@ -4585,7 +6286,7 @@
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="155"/>
       <c r="B22" s="117" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C22" s="118">
         <f>C5</f>
@@ -4631,7 +6332,7 @@
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="155"/>
       <c r="B23" s="117" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C23" s="118">
         <f>C6</f>
@@ -4677,7 +6378,7 @@
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="155"/>
       <c r="B24" s="117" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C24" s="118">
         <f>C7</f>
@@ -4723,7 +6424,7 @@
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="155"/>
       <c r="B25" s="117" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C25" s="118">
         <f>C8</f>
@@ -4782,10 +6483,10 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="155" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B27" s="117" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C27" s="121">
         <f>Ricavi!I94</f>
@@ -4831,7 +6532,7 @@
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="155"/>
       <c r="B28" s="117" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C28" s="121">
         <f>Ricavi!I95</f>
@@ -4877,7 +6578,7 @@
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="155"/>
       <c r="B29" s="117" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C29" s="121">
         <f>Ricavi!I96</f>
@@ -4923,7 +6624,7 @@
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="155"/>
       <c r="B30" s="117" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C30" s="121">
         <f>Ricavi!I97</f>
@@ -4969,7 +6670,7 @@
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="155"/>
       <c r="B31" s="117" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C31" s="121">
         <f>Ricavi!I98</f>
@@ -5029,7 +6730,7 @@
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" s="115"/>
       <c r="B33" s="117" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C33" s="118">
         <f>D4</f>
@@ -5074,7 +6775,7 @@
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B34" s="117" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C34" s="118">
         <f>D5</f>
@@ -5119,7 +6820,7 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B35" s="117" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C35" s="118">
         <f>D6</f>
@@ -5164,7 +6865,7 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B36" s="117" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C36" s="118">
         <f>D7</f>
@@ -5209,7 +6910,7 @@
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B37" s="117" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C37" s="118">
         <f>D8</f>
@@ -5267,7 +6968,7 @@
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B39" s="117" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C39" s="118">
         <f>SUM(C35:C37)</f>
@@ -5312,7 +7013,7 @@
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B40" s="117" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C40" s="118">
         <f>C33</f>
@@ -5357,7 +7058,7 @@
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B41" s="117" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C41" s="118">
         <f>C34</f>
@@ -5402,7 +7103,7 @@
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B42" s="117" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C42" s="123">
         <f>Ricavi!L65 - Ricavi!M66*Ricavi!L66</f>
@@ -5447,7 +7148,7 @@
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B43" s="117" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C43" s="123">
         <v>0</v>
@@ -5501,7 +7202,7 @@
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B45" s="127" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C45" s="123">
         <f xml:space="preserve"> SUM(C39:C43)</f>
@@ -5559,7 +7260,7 @@
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C47" s="123" cm="1">
         <f t="array" ref="C47">-SUM(RicaviBudget!D3:D63*RicaviBudget!F3:F63)</f>
@@ -5604,7 +7305,7 @@
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C48" s="123">
         <v>0</v>
@@ -5659,7 +7360,7 @@
     </row>
     <row r="50" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B50" s="127" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C50" s="123">
         <f>SUM(C47:C48)</f>
@@ -5717,7 +7418,7 @@
     </row>
     <row r="52" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C52" s="128">
         <f>'CE Budget 2022'!C14</f>
@@ -5806,7 +7507,7 @@
     </row>
     <row r="54" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C54" s="128">
         <f>'CE Budget 2022'!C16</f>
@@ -5863,7 +7564,7 @@
     </row>
     <row r="56" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B56" s="127" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C56" s="128">
         <f t="shared" ref="C56:H56" si="12">SUM(C52:C54)</f>
@@ -5921,7 +7622,7 @@
     </row>
     <row r="58" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B58" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C58" s="128">
         <f>'CE Budget 2022'!C18</f>
@@ -5965,7 +7666,7 @@
     </row>
     <row r="59" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B59" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C59" s="128">
         <f>'CE Budget 2022'!C19</f>
@@ -6022,7 +7723,7 @@
     </row>
     <row r="61" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B61" s="127" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C61" s="128">
         <f>SUM(C58+C59)</f>
@@ -6079,7 +7780,7 @@
     </row>
     <row r="63" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B63" s="93" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C63" s="141">
         <f>C45+C50+C56+C61</f>
@@ -6124,7 +7825,7 @@
     </row>
     <row r="64" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B64" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C64" s="128">
         <f>-FixedCostsBudget!C3</f>
@@ -6259,7 +7960,7 @@
     </row>
     <row r="67" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B67" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C67" s="128">
         <f>-FixedCostsBudget!C9</f>
@@ -6304,7 +8005,7 @@
     </row>
     <row r="68" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B68" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C68" s="128">
         <f>-FixedCostsBudget!C11</f>
@@ -6349,7 +8050,7 @@
     </row>
     <row r="69" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B69" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C69" s="128">
         <f>-FixedCostsBudget!C13</f>
@@ -6407,7 +8108,7 @@
     </row>
     <row r="71" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B71" s="127" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C71" s="128">
         <f>SUM(C64:C69)</f>
@@ -6465,7 +8166,7 @@
     </row>
     <row r="73" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B73" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C73" s="128">
         <f>-FixedCostsBudget!C18</f>
@@ -6613,7 +8314,7 @@
     </row>
     <row r="77" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B77" s="127" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C77" s="128">
         <f>SUM(C73:C75)</f>
@@ -6658,7 +8359,7 @@
     </row>
     <row r="78" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B78" s="93" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C78" s="141">
         <f>+C63+C71+C77</f>
@@ -7835,7 +9536,7 @@
       </c>
       <c r="C2" s="147"/>
       <c r="D2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E2" s="146" t="s">
         <v>139</v>
@@ -7844,7 +9545,7 @@
     </row>
     <row r="3" spans="2:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="144" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C3" s="42" t="s">
         <v>65</v>
@@ -7856,7 +9557,7 @@
         <v>65</v>
       </c>
       <c r="P3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="4" spans="2:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -7890,7 +9591,7 @@
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B6" s="46" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C6" s="45">
         <f>SUMIF(RicaviBudget!$H:$H,"MP",RicaviBudget!$G:$G)</f>
@@ -7901,7 +9602,7 @@
         <v>-331642.38355000003</v>
       </c>
       <c r="E6" s="46" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F6" s="45">
         <v>528226.62545000005</v>
@@ -7909,7 +9610,7 @@
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B7" s="44" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C7" s="45">
         <f>SUMIF(RicaviBudget!$H:$H,"PCL",RicaviBudget!$G:$G)</f>
@@ -7920,7 +9621,7 @@
         <v>612028.60988000012</v>
       </c>
       <c r="E7" s="44" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F7" s="45">
         <v>1877590.3519999997</v>
@@ -7982,7 +9683,7 @@
         <v>64320476.000249997</v>
       </c>
       <c r="P10" s="102" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.3">
@@ -8804,16 +10505,16 @@
         <v>200</v>
       </c>
       <c r="F3" s="96" t="s">
+        <v>376</v>
+      </c>
+      <c r="G3" s="96" t="s">
         <v>377</v>
       </c>
-      <c r="G3" s="96" t="s">
-        <v>378</v>
-      </c>
       <c r="H3" s="96" t="s">
+        <v>300</v>
+      </c>
+      <c r="I3" s="96" t="s">
         <v>301</v>
-      </c>
-      <c r="I3" s="96" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -8887,7 +10588,7 @@
       <c r="E6" s="96" t="s">
         <v>209</v>
       </c>
-      <c r="F6" s="158">
+      <c r="F6" s="96">
         <f>'Analisi degli scostamenti'!F25 + 'Analisi degli scostamenti'!F22</f>
         <v>14624209.466660157</v>
       </c>
@@ -9122,22 +10823,22 @@
         <v>200</v>
       </c>
       <c r="F19" s="96" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="G19" s="96" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H19" s="96" t="s">
+        <v>300</v>
+      </c>
+      <c r="I19" s="96" t="s">
         <v>301</v>
-      </c>
-      <c r="I19" s="96" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="96"/>
       <c r="B20" s="96" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C20" s="96">
         <f>VariableCosts!E6</f>
@@ -9167,7 +10868,7 @@
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="96"/>
       <c r="B21" s="96" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C21" s="96">
         <f>VariableCosts!E7</f>
@@ -9432,7 +11133,7 @@
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.3">
       <c r="E39" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.3">
@@ -9514,11 +11215,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:XFD1048576"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" zoomScale="83" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView topLeftCell="A39" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I68" sqref="I68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12451,7 +14152,7 @@
       </c>
       <c r="H69" s="37"/>
       <c r="M69" s="88" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="70" spans="2:17" x14ac:dyDescent="0.3">
@@ -12743,40 +14444,40 @@
     </row>
     <row r="86" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B86" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="87" spans="2:17" x14ac:dyDescent="0.3">
       <c r="K87" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="M87" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="O87" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="Q87" s="1" t="s">
         <v>372</v>
-      </c>
-      <c r="M87" s="1" t="s">
-        <v>371</v>
-      </c>
-      <c r="O87" s="1" t="s">
-        <v>374</v>
-      </c>
-      <c r="Q87" s="1" t="s">
-        <v>373</v>
       </c>
     </row>
     <row r="88" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B88" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C88" s="137">
         <f>SUM(D4:D27)</f>
         <v>240574.55000000005</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F88" s="137" cm="1">
         <f t="array" ref="F88">SUM(D4:D27*E4:E27)</f>
         <v>528226.62545000017</v>
       </c>
       <c r="H88" s="1" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="I88" s="137" cm="1">
         <f t="array" ref="I88">SUM(D4:D27*F4:F27)</f>
@@ -12801,21 +14502,21 @@
     </row>
     <row r="89" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B89" s="1" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C89" s="137">
         <f>SUM(D28:D32)</f>
         <v>3223711</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="F89" s="137" cm="1">
         <f t="array" ref="F89">SUM(D28:D32*E28:E32)</f>
         <v>1877590.3519999997</v>
       </c>
       <c r="H89" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="I89" s="137" cm="1">
         <f t="array" ref="I89">SUM(D28:D32*F28:F32)</f>
@@ -12840,21 +14541,21 @@
     </row>
     <row r="90" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B90" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C90" s="137">
         <f>SUM(D33:D40)</f>
         <v>18642746</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="F90" s="137" cm="1">
         <f t="array" ref="F90">SUM(D33:D40*E33:E40)</f>
         <v>39445016.509999998</v>
       </c>
       <c r="H90" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="I90" s="137" cm="1">
         <f t="array" ref="I90">SUM(D33:D40*F33:F40)</f>
@@ -12879,21 +14580,21 @@
     </row>
     <row r="91" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B91" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C91" s="137">
         <f>SUM(D41:D57)</f>
         <v>6692984</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F91" s="137" cm="1">
         <f t="array" ref="F91">SUM(D41:D57*E41:E57)</f>
         <v>8028278.8500000006</v>
       </c>
       <c r="H91" s="1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="I91" s="137" cm="1">
         <f t="array" ref="I91">SUM(D41:D57*F41:F57)</f>
@@ -12918,21 +14619,21 @@
     </row>
     <row r="92" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B92" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C92" s="137">
         <f>SUM(D58:D76)</f>
         <v>9727258</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="F92" s="137" cm="1">
         <f t="array" ref="F92">SUM(D58:D76*E58:E76)</f>
         <v>13754406.152800001</v>
       </c>
       <c r="H92" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="I92" s="137" cm="1">
         <f t="array" ref="I92">SUM(D58:D76*F58:F76)</f>
@@ -12960,35 +14661,35 @@
       <c r="F93" s="137"/>
       <c r="I93" s="137"/>
       <c r="K93" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="M93" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="O93" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="M93" s="1" t="s">
-        <v>371</v>
-      </c>
-      <c r="O93" s="1" t="s">
-        <v>376</v>
-      </c>
       <c r="Q93" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="94" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B94" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C94" s="137">
         <f>SUM(L4:L17)</f>
         <v>112952.51999999999</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F94" s="137" cm="1">
         <f t="array" ref="F94">SUM(L4:L17*M4:M17)</f>
         <v>196584.24189999999</v>
       </c>
       <c r="H94" s="1" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="I94" s="137" cm="1">
         <f t="array" ref="I94">SUM(L4:L17*O4:O17)</f>
@@ -13013,21 +14714,21 @@
     </row>
     <row r="95" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B95" s="1" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C95" s="137">
         <f>SUM(L18:L22)</f>
         <v>3319903</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="F95" s="137" cm="1">
         <f t="array" ref="F95">SUM(L18:L22*M18:M22)</f>
         <v>2489618.9618799998</v>
       </c>
       <c r="H95" s="1" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="I95" s="137" cm="1">
         <f t="array" ref="I95">SUM(L18:L22*O18:O22)</f>
@@ -13052,21 +14753,21 @@
     </row>
     <row r="96" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B96" s="1" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C96" s="137">
         <f>SUM(L23:L29)</f>
         <v>14624683</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="F96" s="137" cm="1">
         <f t="array" ref="F96">SUM(L23:L29*M23:M29)</f>
         <v>43389917.016709402</v>
       </c>
       <c r="H96" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="I96" s="137" cm="1">
         <f t="array" ref="I96">SUM(L23:L29*O23:O29)</f>
@@ -13091,21 +14792,21 @@
     </row>
     <row r="97" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B97" s="1" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C97" s="137">
         <f>SUM(L30:L45)</f>
         <v>6470002</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="F97" s="137" cm="1">
         <f t="array" ref="F97">SUM(L30:L45*M30:M45)</f>
         <v>9386776.6740170922</v>
       </c>
       <c r="H97" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="I97" s="137" cm="1">
         <f t="array" ref="I97">SUM(L30:L45*O30:O45)</f>
@@ -13130,21 +14831,21 @@
     </row>
     <row r="98" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B98" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C98" s="137">
         <f>SUM(L46:L64)</f>
         <v>9655208.9900000002</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="F98" s="137" cm="1">
         <f t="array" ref="F98">SUM(L46:L64*M46:M64)</f>
         <v>15581855.327799987</v>
       </c>
       <c r="H98" s="1" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="I98" s="137" cm="1">
         <f t="array" ref="I98">SUM(L46:L64*O46:O64)</f>
@@ -13169,7 +14870,7 @@
     </row>
     <row r="100" spans="2:17" x14ac:dyDescent="0.3">
       <c r="E100" s="1" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="F100" s="137" cm="1">
         <f t="array" ref="F100">SUM(L10:L23*M10:M23)</f>
@@ -13179,7 +14880,7 @@
     <row r="101" spans="2:17" x14ac:dyDescent="0.3">
       <c r="C101" s="137"/>
       <c r="E101" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="F101" s="137" cm="1">
         <f t="array" ref="F101">SUM(L24:L28*M24:M28)</f>
@@ -13188,7 +14889,7 @@
     </row>
     <row r="102" spans="2:17" x14ac:dyDescent="0.3">
       <c r="E102" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="F102" s="137" cm="1">
         <f t="array" ref="F102">SUM(L29:L35*M29:M35)</f>
@@ -13197,7 +14898,7 @@
     </row>
     <row r="103" spans="2:17" x14ac:dyDescent="0.3">
       <c r="E103" s="1" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="F103" s="137" cm="1">
         <f t="array" ref="F103">SUM(L36:L51*M36:M51)</f>
@@ -13206,7 +14907,7 @@
     </row>
     <row r="104" spans="2:17" x14ac:dyDescent="0.3">
       <c r="E104" s="1" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="F104" s="137" t="e" cm="1">
         <f t="array" ref="F104">SUM(L52:L70*M52:M70)</f>
@@ -13223,15 +14924,16 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EAEFA6D-2B43-44D4-9785-BA525C9ED11E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EAEFA6D-2B43-44D4-9785-BA525C9ED11E}">
   <dimension ref="A1:L67"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I62" sqref="I62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13273,7 +14975,7 @@
         <v>196</v>
       </c>
       <c r="F2" s="96" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="G2" s="96" t="s">
         <v>197</v>
@@ -13908,7 +15610,7 @@
         <v>204</v>
       </c>
       <c r="I22" s="96" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
@@ -14129,7 +15831,7 @@
         <v>205</v>
       </c>
       <c r="I29" s="96" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="K29" s="96"/>
     </row>
@@ -14913,7 +16615,7 @@
       </c>
       <c r="I54" s="96"/>
       <c r="K54" s="104" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.3">
@@ -14982,7 +16684,7 @@
       </c>
       <c r="I56" s="96"/>
       <c r="K56" s="104" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.3">
@@ -15051,7 +16753,7 @@
       </c>
       <c r="I58" s="96"/>
       <c r="K58" s="104" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.3">
@@ -15231,7 +16933,7 @@
         <v>1</v>
       </c>
       <c r="F64" s="96" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G64" s="96">
         <f t="shared" si="0"/>
@@ -15262,7 +16964,7 @@
         <v>18980.987499999999</v>
       </c>
       <c r="F65" s="96" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G65" s="96">
         <f>-D65*E65</f>
@@ -15303,6 +17005,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -15310,8 +17013,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD57A733-1E5A-4C67-BA94-1CEFC4F75056}">
   <dimension ref="B1:P34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15701,11 +17404,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EB61E9C-EC3D-49DF-83B5-89D531594792}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EB61E9C-EC3D-49DF-83B5-89D531594792}">
   <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15763,10 +17466,10 @@
         <v>212</v>
       </c>
       <c r="H3" s="96" t="s">
+        <v>300</v>
+      </c>
+      <c r="I3" s="96" t="s">
         <v>301</v>
-      </c>
-      <c r="I3" s="96" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -16079,7 +17782,7 @@
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="96"/>
       <c r="B20" s="96" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C20" s="96">
         <f>VariableCosts!E6</f>
@@ -16094,7 +17797,7 @@
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="96"/>
       <c r="B21" s="96" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C21" s="96">
         <f>VariableCosts!E7</f>
@@ -16123,7 +17826,7 @@
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="96"/>
       <c r="B23" s="96" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C23" s="106">
         <f>C22*C21</f>
@@ -16287,6 +17990,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -16430,10 +18134,12 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92EB1E3B-0C1C-4993-9177-FBCEDBD20284}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92EB1E3B-0C1C-4993-9177-FBCEDBD20284}">
   <dimension ref="B2:D27"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -16600,6 +18306,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -16607,7 +18314,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BC74C4D-8FA0-4227-922B-636E2D04E620}">
   <dimension ref="B1:I28"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -16758,11 +18467,11 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D09BE109-08EA-4B02-B169-2F563F62FEDC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D09BE109-08EA-4B02-B169-2F563F62FEDC}">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16933,7 +18642,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>277</v>
+        <v>409</v>
       </c>
       <c r="C23">
         <v>750000</v>
@@ -16941,7 +18650,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C24">
         <v>6.25E-2</v>
@@ -16949,5 +18658,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>